<commit_message>
countries annual net added
</commit_message>
<xml_diff>
--- a/Countries.xlsx
+++ b/Countries.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanjohnston/Development/R/DataMining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darra\OneDrive\Documents\datamining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF94EB5-6919-A743-974C-EC025D583166}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC19E750-66EF-4B18-ABB7-0952010B146C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17360" yWindow="3140" windowWidth="12020" windowHeight="12000" xr2:uid="{683810BD-CB3E-C84B-9895-6EF135447DED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{683810BD-CB3E-C84B-9895-6EF135447DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Country</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Moldova</t>
   </si>
   <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
     <t>Slovenia</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>North Cyprus</t>
-  </si>
-  <si>
     <t>Cyprus</t>
   </si>
   <si>
@@ -193,6 +184,144 @@
   </si>
   <si>
     <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>UZB</t>
+  </si>
+  <si>
+    <t>Sk</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>TKM</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>AZE</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>MNE</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>BIH</t>
+  </si>
+  <si>
+    <t>TJK</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>BG</t>
   </si>
 </sst>
 </file>
@@ -547,19 +676,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E538FD-71AC-7D4C-8809-C831ED2EF0D3}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -573,384 +702,645 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
         <v>4548</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>C2*12</f>
+        <v>54576</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
         <v>3221</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f>C3*12</f>
+        <v>38652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
         <v>3562</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" ref="D4:D47" si="0">C4*12</f>
+        <v>42744</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
         <v>3256</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>39072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
         <v>2509</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>30108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7">
         <v>2240</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>26880</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
         <v>2822</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>33864</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
         <v>2740</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
         <v>3573</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>42876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11">
         <v>2748</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>32976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12">
         <v>2262</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>27144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2531</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>30372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14">
-        <v>2531</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1106</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>13272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1784</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>21408</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1021</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>12252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>851</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>10212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1729</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>20748</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1328</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>15936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
       <c r="C22">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+        <v>967</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>11604</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="C23">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>10560</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="C25">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+        <v>942</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>11304</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
       <c r="C26">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>5388</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1658</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>19896</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C29">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
       <c r="C30">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1214</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>14568</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33">
-        <v>1214</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+        <v>527</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>6324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
       <c r="B34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>743</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>8916</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
       <c r="B35" t="s">
         <v>37</v>
       </c>
       <c r="C35">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+        <v>562</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>6744</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
       <c r="C36">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1004</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>12048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
       <c r="C37">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+        <v>915</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>10980</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
       <c r="C38">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>5232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
       <c r="C39">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>4272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
       <c r="B40" t="s">
         <v>42</v>
       </c>
       <c r="C40">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+        <v>492</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>5904</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
       <c r="B41" t="s">
         <v>43</v>
       </c>
       <c r="C41">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+        <v>1116</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>13392</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
       <c r="B42" t="s">
         <v>44</v>
       </c>
       <c r="C42">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+        <v>755</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>9060</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
       <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
       <c r="B44" t="s">
         <v>46</v>
       </c>
       <c r="C44">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>4044</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
       <c r="B45" t="s">
         <v>47</v>
       </c>
-      <c r="C45">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
       <c r="B47" t="s">
         <v>49</v>
       </c>
       <c r="C47">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50">
         <v>554</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>6648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>